<commit_message>
Added GitHub link to BOM
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Printlab_Beverage_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Printlab_Beverage_Can_Opener_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Jason@Printlabs_Beverage_Can_Opener/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Printlab_Beverage_Can_Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E85C0B02-7A38-430C-A22D-FE9ADE615562}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94EA3C73-0FC4-4A0C-9B38-8B82FCDF2BF0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,10 +116,10 @@
     <t>The fully funtional Beverage Can Opener from Printlab, in a single piece.</t>
   </si>
   <si>
-    <t>Add GitHub Link</t>
-  </si>
-  <si>
     <t>Total Print Cost:</t>
+  </si>
+  <si>
+    <t>https://github.com/makersmakingchange/Printlab_Beverage_Can_Opener/tree/main/Build_Files/3D_Print_Files</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,7 +682,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G7" dT="2022-06-08T14:39:18.50" personId="{61C8B5B5-DE08-4776-8DB0-B040ED353EF5}" id="{A4F02849-0FFE-48E7-A231-975A4B56DA31}">
+  <threadedComment ref="G7" dT="2022-06-08T14:39:18.50" personId="{61C8B5B5-DE08-4776-8DB0-B040ED353EF5}" id="{A4F02849-0FFE-48E7-A231-975A4B56DA31}" done="1">
     <text>Just commenting as a reminder for the github link</text>
   </threadedComment>
 </ThreadedComments>
@@ -693,25 +693,25 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="75.6640625" customWidth="1"/>
     <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="89.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.9">
+    <row r="1" spans="1:12" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -725,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -745,12 +745,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="22"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>6</v>
       </c>
@@ -762,7 +762,7 @@
       <c r="G5" s="18"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -785,7 +785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="31.9" customHeight="1">
+    <row r="7" spans="1:12" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -806,13 +806,13 @@
         <v>38</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="D8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="16">
         <f>SUM(E7:E7)</f>
@@ -821,33 +821,16 @@
       <c r="G8" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1" xr:uid="{7F39AB56-749B-4E87-BD49-D6A2F180A333}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100456CAEA290209545A9F8681F83603874" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d27786a72e09a52c769a64d5f7eeaa24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cf100d1-0775-4feb-8634-62999c4541bc" xmlns:ns3="38b325e6-602c-452a-8617-173bf47082c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03ae89856d271009074f70b56337b48d" ns2:_="" ns3:_="">
     <xsd:import namespace="8cf100d1-0775-4feb-8634-62999c4541bc"/>
@@ -1084,14 +1067,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99BECD52-63A8-454F-82E6-6195B786F95C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99BECD52-63A8-454F-82E6-6195B786F95C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>